<commit_message>
fixed elective slot naming
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -81,12 +81,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A8D5BA"/>
-        <bgColor rgb="00A8D5BA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FFFACD"/>
         <bgColor rgb="00FFFACD"/>
       </patternFill>
@@ -107,6 +101,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00B0C4DE"/>
         <bgColor rgb="00B0C4DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A8D5BA"/>
+        <bgColor rgb="00A8D5BA"/>
       </patternFill>
     </fill>
     <fill>
@@ -242,19 +242,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -793,18 +793,16 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>B1-IOT101 LEC
-C101
-Dr Jagadeesha Bhat</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>B2-IIP101 LEC
-C104
-Mr. Ram Subramanian &amp; Mr. Sasi Kumar Sundara Rajan</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F2" s="4" t="n"/>
@@ -822,31 +820,31 @@
       </c>
       <c r="K2" s="9" t="inlineStr">
         <is>
-          <t>CS162 LEC
+          <t>CS165 LEC
 C101
-Dr. Dibyajyothi</t>
+Dr. Animesh Roy</t>
         </is>
       </c>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="5" t="n"/>
       <c r="N2" s="10" t="inlineStr">
         <is>
-          <t>CS165 LEC
-C101
-Dr. Animesh Roy</t>
-        </is>
-      </c>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="5" t="n"/>
-      <c r="Q2" s="11" t="inlineStr">
-        <is>
           <t>HS204  LEC
 C101
 Dr. Anusree Kini</t>
         </is>
       </c>
-      <c r="R2" s="4" t="n"/>
-      <c r="S2" s="5" t="n"/>
+      <c r="O2" s="4" t="n"/>
+      <c r="P2" s="5" t="n"/>
+      <c r="Q2" s="10" t="inlineStr">
+        <is>
+          <t>HS204  TUT
+C101
+Dr. Anusree Kini</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="n"/>
+      <c r="S2" s="7" t="inlineStr"/>
       <c r="T2" s="7" t="inlineStr"/>
     </row>
     <row r="3" ht="40" customHeight="1">
@@ -857,18 +855,16 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>B1-IOT101 LEC
-C101
-Dr Jagadeesha Bhat</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="5" t="n"/>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>B2-IIP101 LEC
-C104
-Mr. Ram Subramanian &amp; Mr. Sasi Kumar Sundara Rajan</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F3" s="4" t="n"/>
@@ -884,7 +880,7 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K3" s="12" t="inlineStr">
+      <c r="K3" s="11" t="inlineStr">
         <is>
           <t>CS163 LEC
 C101
@@ -895,23 +891,23 @@
       <c r="M3" s="5" t="n"/>
       <c r="N3" s="12" t="inlineStr">
         <is>
-          <t>CS163 LAB
-C101
-Prof. CB Akki/Dr. Suvadip Hazra</t>
-        </is>
-      </c>
-      <c r="O3" s="4" t="n"/>
-      <c r="P3" s="4" t="n"/>
-      <c r="Q3" s="5" t="n"/>
-      <c r="R3" s="13" t="inlineStr">
-        <is>
           <t>CS164 LEC
 C101
 Dr. Prabhu Prasad/Prof. CB Akki</t>
         </is>
       </c>
-      <c r="S3" s="4" t="n"/>
-      <c r="T3" s="5" t="n"/>
+      <c r="O3" s="4" t="n"/>
+      <c r="P3" s="5" t="n"/>
+      <c r="Q3" s="12" t="inlineStr">
+        <is>
+          <t>CS164 LEC
+C101
+Dr. Prabhu Prasad/Prof. CB Akki</t>
+        </is>
+      </c>
+      <c r="R3" s="4" t="n"/>
+      <c r="S3" s="5" t="n"/>
+      <c r="T3" s="7" t="inlineStr"/>
     </row>
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -921,18 +917,16 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>B1-IOT101 LEC
-C101
-Dr Jagadeesha Bhat</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="5" t="n"/>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>B2-IIP101 LEC
-C104
-Mr. Ram Subramanian &amp; Mr. Sasi Kumar Sundara Rajan</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F4" s="4" t="n"/>
@@ -948,24 +942,18 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K4" s="13" t="inlineStr">
-        <is>
-          <t>CS164 LAB
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>CS165 LEC
 C101
-Dr. Prabhu Prasad/Prof. CB Akki</t>
+Dr. Animesh Roy</t>
         </is>
       </c>
       <c r="L4" s="4" t="n"/>
-      <c r="M4" s="4" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="11" t="inlineStr">
-        <is>
-          <t>HS204  TUT
-C101
-Dr. Anusree Kini</t>
-        </is>
-      </c>
-      <c r="P4" s="5" t="n"/>
+      <c r="M4" s="5" t="n"/>
+      <c r="N4" s="7" t="inlineStr"/>
+      <c r="O4" s="7" t="inlineStr"/>
+      <c r="P4" s="7" t="inlineStr"/>
       <c r="Q4" s="7" t="inlineStr"/>
       <c r="R4" s="7" t="inlineStr"/>
       <c r="S4" s="7" t="inlineStr"/>
@@ -979,18 +967,16 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>B1-IOT101 LEC
-C101
-Dr Jagadeesha Bhat</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
       <c r="E5" s="6" t="inlineStr">
         <is>
-          <t>B2-IIP101 LEC
-C104
-Mr. Ram Subramanian &amp; Mr. Sasi Kumar Sundara Rajan</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F5" s="4" t="n"/>
@@ -1006,28 +992,34 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K5" s="12" t="inlineStr">
+      <c r="K5" s="13" t="inlineStr">
+        <is>
+          <t>CS162 LEC
+C101
+Dr. Dibyajyothi</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="n"/>
+      <c r="M5" s="5" t="n"/>
+      <c r="N5" s="11" t="inlineStr">
         <is>
           <t>CS163 LEC
 C101
 Prof. CB Akki/Dr. Suvadip Hazra</t>
         </is>
       </c>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="10" t="inlineStr">
-        <is>
-          <t>CS165 LEC
-C101
-Dr. Animesh Roy</t>
-        </is>
-      </c>
       <c r="O5" s="4" t="n"/>
       <c r="P5" s="5" t="n"/>
-      <c r="Q5" s="7" t="inlineStr"/>
-      <c r="R5" s="7" t="inlineStr"/>
-      <c r="S5" s="7" t="inlineStr"/>
-      <c r="T5" s="7" t="inlineStr"/>
+      <c r="Q5" s="11" t="inlineStr">
+        <is>
+          <t>CS163 LAB
+C101
+Prof. CB Akki/Dr. Suvadip Hazra</t>
+        </is>
+      </c>
+      <c r="R5" s="4" t="n"/>
+      <c r="S5" s="4" t="n"/>
+      <c r="T5" s="5" t="n"/>
     </row>
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -1037,18 +1029,16 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>B1-IOT101 LEC
-C101
-Dr Jagadeesha Bhat</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>B2-IIP101 LEC
-C104
-Mr. Ram Subramanian &amp; Mr. Sasi Kumar Sundara Rajan</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F6" s="4" t="n"/>
@@ -1064,7 +1054,7 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K6" s="9" t="inlineStr">
+      <c r="K6" s="13" t="inlineStr">
         <is>
           <t>CS162 LEC
 C101
@@ -1073,7 +1063,7 @@
       </c>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="5" t="n"/>
-      <c r="N6" s="9" t="inlineStr">
+      <c r="N6" s="13" t="inlineStr">
         <is>
           <t>CS162 TUT
 C101
@@ -1081,16 +1071,16 @@
         </is>
       </c>
       <c r="O6" s="5" t="n"/>
-      <c r="P6" s="13" t="inlineStr">
-        <is>
-          <t>CS164 LEC
+      <c r="P6" s="12" t="inlineStr">
+        <is>
+          <t>CS164 LAB
 C101
 Dr. Prabhu Prasad/Prof. CB Akki</t>
         </is>
       </c>
       <c r="Q6" s="4" t="n"/>
-      <c r="R6" s="5" t="n"/>
-      <c r="S6" s="7" t="inlineStr"/>
+      <c r="R6" s="4" t="n"/>
+      <c r="S6" s="5" t="n"/>
       <c r="T6" s="7" t="inlineStr"/>
     </row>
     <row r="9">
@@ -1345,24 +1335,24 @@
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="Q2:S2"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="P6:S6"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="Q5:T5"/>
     <mergeCell ref="K3:M3"/>
+    <mergeCell ref="Q3:S3"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1512,9 +1502,15 @@
           <t>Monday</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr"/>
-      <c r="C2" s="7" t="inlineStr"/>
-      <c r="D2" s="7" t="inlineStr"/>
+      <c r="B2" s="13" t="inlineStr">
+        <is>
+          <t>CS307 LEC
+L305
+Dr. Rajib Sharma/ Dr. Rao (Lab)</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="5" t="n"/>
       <c r="E2" s="7" t="inlineStr"/>
       <c r="F2" s="7" t="inlineStr"/>
       <c r="G2" s="7" t="inlineStr"/>
@@ -1530,11 +1526,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L2" s="12" t="inlineStr">
-        <is>
-          <t>B4 LEC
-L301
-Dr. Girish G N</t>
+      <c r="L2" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M2" s="4" t="n"/>
@@ -1552,15 +1547,15 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> B4-DS351 TUT
-L303
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> B4-DS351 LEC
+L305
 Dr. Ramesh Athe</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n"/>
-      <c r="D3" s="7" t="inlineStr"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="5" t="n"/>
       <c r="E3" s="7" t="inlineStr"/>
       <c r="F3" s="7" t="inlineStr"/>
       <c r="G3" s="7" t="inlineStr"/>
@@ -1576,11 +1571,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L3" s="12" t="inlineStr">
-        <is>
-          <t>B4 LEC
-L303
-Dr. Girish G N</t>
+      <c r="L3" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M3" s="4" t="n"/>
@@ -1598,24 +1592,12 @@
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>CS307 LEC
-L304
-Dr. Rajib Sharma/ Dr. Rao (Lab)</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> B4-DS351 LEC
-L403
-Dr. Ramesh Athe</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="n"/>
-      <c r="G4" s="5" t="n"/>
+      <c r="B4" s="7" t="inlineStr"/>
+      <c r="C4" s="7" t="inlineStr"/>
+      <c r="D4" s="7" t="inlineStr"/>
+      <c r="E4" s="7" t="inlineStr"/>
+      <c r="F4" s="7" t="inlineStr"/>
+      <c r="G4" s="7" t="inlineStr"/>
       <c r="H4" s="7" t="inlineStr"/>
       <c r="I4" s="7" t="inlineStr"/>
       <c r="J4" s="8" t="inlineStr">
@@ -1628,11 +1610,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L4" s="12" t="inlineStr">
-        <is>
-          <t>B4 LEC
-L302
-Dr. Girish G N</t>
+      <c r="L4" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M4" s="4" t="n"/>
@@ -1650,24 +1631,24 @@
           <t>Thursday</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>CS307 SS
+      <c r="B5" s="13" t="inlineStr">
+        <is>
+          <t>CS307 LEC
 L304
 Dr. Rajib Sharma/ Dr. Rao (Lab)</t>
         </is>
       </c>
-      <c r="C5" s="5" t="n"/>
-      <c r="D5" s="13" t="inlineStr">
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="5" t="n"/>
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> B4-DS351 LEC
-L403
+L402
 Dr. Ramesh Athe</t>
         </is>
       </c>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="7" t="inlineStr"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="5" t="n"/>
       <c r="H5" s="7" t="inlineStr"/>
       <c r="I5" s="7" t="inlineStr"/>
       <c r="J5" s="8" t="inlineStr">
@@ -1680,11 +1661,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L5" s="12" t="inlineStr">
-        <is>
-          <t>B4 LEC
-L304
-Dr. Girish G N</t>
+      <c r="L5" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M5" s="4" t="n"/>
@@ -1702,16 +1682,22 @@
           <t>Friday</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>CS307 LEC
-L305
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>CS307 SS
+L304
 Dr. Rajib Sharma/ Dr. Rao (Lab)</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="5" t="n"/>
-      <c r="E6" s="7" t="inlineStr"/>
+      <c r="C6" s="5" t="n"/>
+      <c r="D6" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> B4-DS351 TUT
+L402
+Dr. Ramesh Athe</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="n"/>
       <c r="F6" s="7" t="inlineStr"/>
       <c r="G6" s="7" t="inlineStr"/>
       <c r="H6" s="7" t="inlineStr"/>
@@ -1726,11 +1712,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L6" s="12" t="inlineStr">
-        <is>
-          <t>B4 LEC
-C204
-Dr. Girish G N</t>
+      <c r="L6" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M6" s="4" t="n"/>
@@ -1784,17 +1769,17 @@
     <row r="12">
       <c r="A12" s="16" t="inlineStr">
         <is>
-          <t>B1-CS464</t>
+          <t>B2-CS455</t>
         </is>
       </c>
       <c r="B12" s="16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Deep Learning for Computer Vision </t>
+          <t>Blockchain Technology</t>
         </is>
       </c>
       <c r="C12" s="16" t="inlineStr">
         <is>
-          <t>Dr. Chinmayanand</t>
+          <t>Dr. Rajendra H</t>
         </is>
       </c>
       <c r="D12" s="16" t="inlineStr">
@@ -1814,17 +1799,17 @@
     <row r="13">
       <c r="A13" s="16" t="inlineStr">
         <is>
-          <t>B1-NEW</t>
+          <t>B2-EC361</t>
         </is>
       </c>
       <c r="B13" s="16" t="inlineStr">
         <is>
-          <t>Large Languange Models</t>
+          <t>Introduction to 5G Network</t>
         </is>
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>Dr. Sunil S</t>
+          <t>Dr. Jagadeesha R Bhat</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1844,17 +1829,17 @@
     <row r="14">
       <c r="A14" s="16" t="inlineStr">
         <is>
-          <t>B1-CS458</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="B14" s="16" t="inlineStr">
         <is>
-          <t>Natural Language Processing</t>
+          <t>Model Checking</t>
         </is>
       </c>
       <c r="C14" s="16" t="inlineStr">
         <is>
-          <t>Dr. Krishnendu</t>
+          <t>Dr. Pavan</t>
         </is>
       </c>
       <c r="D14" s="16" t="inlineStr">
@@ -1874,17 +1859,17 @@
     <row r="15">
       <c r="A15" s="16" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1-CS464</t>
         </is>
       </c>
       <c r="B15" s="16" t="inlineStr">
         <is>
-          <t>Model Checking</t>
+          <t xml:space="preserve">Deep Learning for Computer Vision </t>
         </is>
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>Dr. Pavan</t>
+          <t>Dr. Chinmayanand</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
@@ -1904,17 +1889,17 @@
     <row r="16">
       <c r="A16" s="16" t="inlineStr">
         <is>
-          <t>B2-NEW</t>
+          <t>B1-CS458</t>
         </is>
       </c>
       <c r="B16" s="16" t="inlineStr">
         <is>
-          <t>Design Thinking and Innovation</t>
+          <t>Natural Language Processing</t>
         </is>
       </c>
       <c r="C16" s="16" t="inlineStr">
         <is>
-          <t>Dr. Sandesh P</t>
+          <t>Dr. Krishnendu</t>
         </is>
       </c>
       <c r="D16" s="16" t="inlineStr">
@@ -1934,17 +1919,17 @@
     <row r="17">
       <c r="A17" s="16" t="inlineStr">
         <is>
-          <t>B2-CS455</t>
+          <t>B1-NEW</t>
         </is>
       </c>
       <c r="B17" s="16" t="inlineStr">
         <is>
-          <t>Blockchain Technology</t>
+          <t>Large Languange Models</t>
         </is>
       </c>
       <c r="C17" s="16" t="inlineStr">
         <is>
-          <t>Dr. Rajendra H</t>
+          <t>Dr. Sunil S</t>
         </is>
       </c>
       <c r="D17" s="16" t="inlineStr">
@@ -1964,17 +1949,17 @@
     <row r="18">
       <c r="A18" s="16" t="inlineStr">
         <is>
-          <t>B2-EC361</t>
+          <t>B2-NEW</t>
         </is>
       </c>
       <c r="B18" s="16" t="inlineStr">
         <is>
-          <t>Introduction to 5G Network</t>
+          <t>Design Thinking and Innovation</t>
         </is>
       </c>
       <c r="C18" s="16" t="inlineStr">
         <is>
-          <t>Dr. Jagadeesha R Bhat</t>
+          <t>Dr. Sandesh P</t>
         </is>
       </c>
       <c r="D18" s="16" t="inlineStr">
@@ -2293,16 +2278,16 @@
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="E4:G4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2812,32 +2797,32 @@
           <t>Monday</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
-        <is>
-          <t>MA202 TUT
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>CS206 TUT
 C102
-Dr. Anand Barangi</t>
+Dr. Pavan/Dr. Sunil C K</t>
         </is>
       </c>
       <c r="C2" s="5" t="n"/>
-      <c r="D2" s="13" t="inlineStr">
-        <is>
-          <t>CS204 LEC
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>CS310 TUT
 C201
-Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="n"/>
-      <c r="F2" s="5" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>CS301 LEC
+Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="n"/>
+      <c r="F2" s="25" t="inlineStr">
+        <is>
+          <t>HS205 LEC
 C201
-Dr. Vivekraj/Dr. Sunil Kumar P V</t>
-        </is>
-      </c>
-      <c r="H2" s="4" t="n"/>
-      <c r="I2" s="5" t="n"/>
+Dr. Jolly Thomas, IIT Dharwad</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="7" t="inlineStr"/>
       <c r="J2" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -2848,16 +2833,10 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L2" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LAB
-C102
-Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
-        </is>
-      </c>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="4" t="n"/>
-      <c r="O2" s="5" t="n"/>
+      <c r="L2" s="7" t="inlineStr"/>
+      <c r="M2" s="7" t="inlineStr"/>
+      <c r="N2" s="7" t="inlineStr"/>
+      <c r="O2" s="7" t="inlineStr"/>
       <c r="P2" s="7" t="inlineStr"/>
       <c r="Q2" s="7" t="inlineStr"/>
       <c r="R2" s="7" t="inlineStr"/>
@@ -2870,25 +2849,25 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t>CS204 LAB
-C201
-Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="4" t="n"/>
-      <c r="E3" s="5" t="n"/>
-      <c r="F3" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LEC
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>CS301 TUT
+C102
+Dr. Vivekraj/Dr. Sunil Kumar P V</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n"/>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LAB
 C201
 Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
         </is>
       </c>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="5" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="7" t="inlineStr"/>
       <c r="I3" s="7" t="inlineStr"/>
       <c r="J3" s="8" t="inlineStr">
         <is>
@@ -2900,23 +2879,11 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L3" s="11" t="inlineStr">
-        <is>
-          <t>CS310 TUT
-C102
-Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
-        </is>
-      </c>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="25" t="inlineStr">
-        <is>
-          <t>HS205 LEC
-C102
-Dr. Jolly Thomas, IIT Dharwad</t>
-        </is>
-      </c>
-      <c r="O3" s="4" t="n"/>
-      <c r="P3" s="5" t="n"/>
+      <c r="L3" s="7" t="inlineStr"/>
+      <c r="M3" s="7" t="inlineStr"/>
+      <c r="N3" s="7" t="inlineStr"/>
+      <c r="O3" s="7" t="inlineStr"/>
+      <c r="P3" s="7" t="inlineStr"/>
       <c r="Q3" s="7" t="inlineStr"/>
       <c r="R3" s="7" t="inlineStr"/>
       <c r="S3" s="7" t="inlineStr"/>
@@ -2928,72 +2895,78 @@
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>CS206 TUT
-C102
-Dr. Pavan/Dr. Sunil C K</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n"/>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>CS204 LEC
-C201
-Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="n"/>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
-        <is>
-          <t>CS301 TUT
-C201
-Dr. Vivekraj/Dr. Sunil Kumar P V</t>
-        </is>
-      </c>
-      <c r="H4" s="5" t="n"/>
-      <c r="I4" s="7" t="inlineStr"/>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="L4" s="7" t="inlineStr"/>
-      <c r="M4" s="7" t="inlineStr"/>
-      <c r="N4" s="7" t="inlineStr"/>
-      <c r="O4" s="7" t="inlineStr"/>
-      <c r="P4" s="7" t="inlineStr"/>
-      <c r="Q4" s="7" t="inlineStr"/>
-      <c r="R4" s="7" t="inlineStr"/>
-      <c r="S4" s="7" t="inlineStr"/>
-      <c r="T4" s="7" t="inlineStr"/>
-    </row>
-    <row r="5" ht="40" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B4" s="13" t="inlineStr">
         <is>
           <t>MA202 LEC
 C102
 Dr. Anand Barangi</t>
         </is>
       </c>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>CS206 LEC
+C201
+Dr. Pavan/Dr. Sunil C K</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="7" t="inlineStr"/>
+      <c r="I4" s="7" t="inlineStr"/>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="L4" s="12" t="inlineStr">
+        <is>
+          <t>CS204 LEC
+C102
+Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
+        </is>
+      </c>
+      <c r="M4" s="4" t="n"/>
+      <c r="N4" s="5" t="n"/>
+      <c r="O4" s="12" t="inlineStr">
+        <is>
+          <t>CS204 LAB
+C101
+Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
+        </is>
+      </c>
+      <c r="P4" s="4" t="n"/>
+      <c r="Q4" s="4" t="n"/>
+      <c r="R4" s="5" t="n"/>
+      <c r="S4" s="7" t="inlineStr"/>
+      <c r="T4" s="7" t="inlineStr"/>
+    </row>
+    <row r="5" ht="40" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>CS204 LEC
+C102
+Dr. Suvadip Hazra/Dr. Malay and Dr. Dibyajyothi</t>
+        </is>
+      </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>MA202 LEC
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LEC
 C201
-Dr. Anand Barangi</t>
+Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
         </is>
       </c>
       <c r="F5" s="4" t="n"/>
@@ -3010,33 +2983,21 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L5" s="12" t="inlineStr">
-        <is>
-          <t>CS206 LEC
+      <c r="L5" s="25" t="inlineStr">
+        <is>
+          <t>HS205 LEC
 C102
-Dr. Pavan/Dr. Sunil C K</t>
+Dr. Jolly Thomas, IIT Dharwad</t>
         </is>
       </c>
       <c r="M5" s="4" t="n"/>
       <c r="N5" s="5" t="n"/>
-      <c r="O5" s="12" t="inlineStr">
-        <is>
-          <t>CS206 LEC
-C102
-Dr. Pavan/Dr. Sunil C K</t>
-        </is>
-      </c>
-      <c r="P5" s="4" t="n"/>
-      <c r="Q5" s="5" t="n"/>
-      <c r="R5" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LEC
-C101
-Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
-        </is>
-      </c>
-      <c r="S5" s="4" t="n"/>
-      <c r="T5" s="5" t="n"/>
+      <c r="O5" s="7" t="inlineStr"/>
+      <c r="P5" s="7" t="inlineStr"/>
+      <c r="Q5" s="7" t="inlineStr"/>
+      <c r="R5" s="7" t="inlineStr"/>
+      <c r="S5" s="7" t="inlineStr"/>
+      <c r="T5" s="7" t="inlineStr"/>
     </row>
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -3044,45 +3005,69 @@
           <t>Friday</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>MA202 LEC
+C102
+Dr. Anand Barangi</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="5" t="n"/>
+      <c r="E6" s="13" t="inlineStr">
+        <is>
+          <t>MA202 TUT
+C201
+Dr. Anand Barangi</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="11" t="inlineStr">
+        <is>
+          <t>CS206 LEC
+C201
+Dr. Pavan/Dr. Sunil C K</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="5" t="n"/>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>CS301 LEC
 C102
 Dr. Vivekraj/Dr. Sunil Kumar P V</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="5" t="n"/>
-      <c r="E6" s="25" t="inlineStr">
-        <is>
-          <t>HS205 LEC
-C201
-Dr. Jolly Thomas, IIT Dharwad</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="5" t="n"/>
-      <c r="H6" s="7" t="inlineStr"/>
-      <c r="I6" s="7" t="inlineStr"/>
-      <c r="J6" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K6" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="L6" s="7" t="inlineStr"/>
-      <c r="M6" s="7" t="inlineStr"/>
-      <c r="N6" s="7" t="inlineStr"/>
-      <c r="O6" s="7" t="inlineStr"/>
-      <c r="P6" s="7" t="inlineStr"/>
-      <c r="Q6" s="7" t="inlineStr"/>
-      <c r="R6" s="7" t="inlineStr"/>
-      <c r="S6" s="7" t="inlineStr"/>
-      <c r="T6" s="7" t="inlineStr"/>
+      <c r="M6" s="4" t="n"/>
+      <c r="N6" s="5" t="n"/>
+      <c r="O6" s="9" t="inlineStr">
+        <is>
+          <t>CS301 LEC
+C102
+Dr. Vivekraj/Dr. Sunil Kumar P V</t>
+        </is>
+      </c>
+      <c r="P6" s="4" t="n"/>
+      <c r="Q6" s="5" t="n"/>
+      <c r="R6" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LEC
+C102
+Dr. Pramod Yelmewad/Dr. Abdul Wahid</t>
+        </is>
+      </c>
+      <c r="S6" s="4" t="n"/>
+      <c r="T6" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="14" t="inlineStr">
@@ -3223,24 +3208,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G4:H4"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L6:N6"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R6:T6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3392,18 +3377,16 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>B1-abc003 LEC
-C204
-Prof. SRM Prasanna</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>B2-abc010 LEC
-L302
-Dr. Sandesh P</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F2" s="4" t="n"/>
@@ -3422,17 +3405,16 @@
       </c>
       <c r="L2" s="26" t="inlineStr">
         <is>
-          <t>B4-abc015 LEC
-C202
-Dr. Girish GN</t>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M2" s="4" t="n"/>
       <c r="N2" s="5" t="n"/>
-      <c r="O2" s="9" t="inlineStr">
+      <c r="O2" s="13" t="inlineStr">
         <is>
           <t>CS307 LEC
-C104
+C102
 Dr. Girish GN/Dr. Krishnendu Ghosh</t>
         </is>
       </c>
@@ -3450,18 +3432,16 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>B1-abc003 LEC
-C203
-Prof. SRM Prasanna</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="5" t="n"/>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>B2-abc010 LEC
-L302
-Dr. Sandesh P</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F3" s="4" t="n"/>
@@ -3480,17 +3460,16 @@
       </c>
       <c r="L3" s="26" t="inlineStr">
         <is>
-          <t>B4-abc015 LEC
-C202
-Dr. Girish GN</t>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M3" s="4" t="n"/>
       <c r="N3" s="5" t="n"/>
-      <c r="O3" s="9" t="inlineStr">
+      <c r="O3" s="13" t="inlineStr">
         <is>
           <t>CS307 LAB
-C104
+C102
 Dr. Girish GN/Dr. Krishnendu Ghosh</t>
         </is>
       </c>
@@ -3508,18 +3487,16 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>B1-abc003 LEC
-C204
-Prof. SRM Prasanna</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="5" t="n"/>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>B2-abc010 LEC
-L302
-Dr. Sandesh P</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F4" s="4" t="n"/>
@@ -3538,22 +3515,15 @@
       </c>
       <c r="L4" s="26" t="inlineStr">
         <is>
-          <t>B4-abc015 LEC
-C201
-Dr. Girish GN</t>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M4" s="4" t="n"/>
       <c r="N4" s="5" t="n"/>
-      <c r="O4" s="9" t="inlineStr">
-        <is>
-          <t>CS307 LEC
-C102
-Dr. Girish GN/Dr. Krishnendu Ghosh</t>
-        </is>
-      </c>
-      <c r="P4" s="4" t="n"/>
-      <c r="Q4" s="5" t="n"/>
+      <c r="O4" s="7" t="inlineStr"/>
+      <c r="P4" s="7" t="inlineStr"/>
+      <c r="Q4" s="7" t="inlineStr"/>
       <c r="R4" s="7" t="inlineStr"/>
       <c r="S4" s="7" t="inlineStr"/>
       <c r="T4" s="7" t="inlineStr"/>
@@ -3566,18 +3536,16 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>B1-abc003 LEC
-C203
-Prof. SRM Prasanna</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
       <c r="E5" s="6" t="inlineStr">
         <is>
-          <t>B2-abc010 LEC
-L302
-Dr. Sandesh P</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F5" s="4" t="n"/>
@@ -3596,9 +3564,8 @@
       </c>
       <c r="L5" s="26" t="inlineStr">
         <is>
-          <t>B4-abc015 LEC
-C202
-Dr. Girish GN</t>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M5" s="4" t="n"/>
@@ -3618,18 +3585,16 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>B1-abc003 LEC
-C203
-Prof. SRM Prasanna</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>B2-abc010 LEC
-L302
-Dr. Sandesh P</t>
+          <t xml:space="preserve">B2 LEC
+</t>
         </is>
       </c>
       <c r="F6" s="4" t="n"/>
@@ -3648,16 +3613,21 @@
       </c>
       <c r="L6" s="26" t="inlineStr">
         <is>
-          <t>B4-abc015 LEC
-C201
-Dr. Girish GN</t>
+          <t xml:space="preserve">B4 LEC
+</t>
         </is>
       </c>
       <c r="M6" s="4" t="n"/>
       <c r="N6" s="5" t="n"/>
-      <c r="O6" s="7" t="inlineStr"/>
-      <c r="P6" s="7" t="inlineStr"/>
-      <c r="Q6" s="7" t="inlineStr"/>
+      <c r="O6" s="13" t="inlineStr">
+        <is>
+          <t>CS307 LEC
+C104
+Dr. Girish GN/Dr. Krishnendu Ghosh</t>
+        </is>
+      </c>
+      <c r="P6" s="4" t="n"/>
+      <c r="Q6" s="5" t="n"/>
       <c r="R6" s="7" t="inlineStr"/>
       <c r="S6" s="7" t="inlineStr"/>
       <c r="T6" s="7" t="inlineStr"/>
@@ -4075,9 +4045,9 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="O4:Q4"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="L5:N5"/>
@@ -4607,10 +4577,16 @@
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
-      <c r="E2" s="7" t="inlineStr"/>
-      <c r="F2" s="7" t="inlineStr"/>
-      <c r="G2" s="7" t="inlineStr"/>
-      <c r="H2" s="7" t="inlineStr"/>
+      <c r="E2" s="25" t="inlineStr">
+        <is>
+          <t>DS164 LAB
+L303
+Dr. Siddharth R</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="n"/>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="5" t="n"/>
       <c r="I2" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -4638,22 +4614,22 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>MA163 LEC
+C205
+Dr. Sibasankar Padhy</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="5" t="n"/>
+      <c r="E3" s="13" t="inlineStr">
         <is>
           <t>MA163 TUT
-C204
+L303
 Dr. Sibasankar Padhy</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n"/>
-      <c r="D3" s="12" t="inlineStr">
-        <is>
-          <t>CS162 LEC
-L303
-Dr. Dibyajyothi Guha</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="n"/>
       <c r="G3" s="7" t="inlineStr"/>
       <c r="H3" s="7" t="inlineStr"/>
@@ -4669,17 +4645,17 @@
       </c>
       <c r="K3" s="11" t="inlineStr">
         <is>
-          <t>CS163 LEC
-C203
-Dr. Sunil Saumya</t>
+          <t>CS162 LEC
+C202
+Dr. Dibyajyothi Guha</t>
         </is>
       </c>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="5" t="n"/>
-      <c r="N3" s="11" t="inlineStr">
+      <c r="N3" s="10" t="inlineStr">
         <is>
           <t>CS163 LAB
-C203
+C202
 Dr. Sunil Saumya</t>
         </is>
       </c>
@@ -4698,80 +4674,80 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>CS164 LAB
-L303
-Dr. Manjunath</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="4" t="n"/>
-      <c r="E4" s="5" t="n"/>
-      <c r="F4" s="10" t="inlineStr">
-        <is>
-          <t>HS161 LEC
-L303
-Dr. Rajesh N S</t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="n"/>
-      <c r="H4" s="5" t="n"/>
-      <c r="I4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K4" s="11" t="inlineStr">
-        <is>
-          <t>CS163 LEC
-C202
-Dr. Sunil Saumya</t>
-        </is>
-      </c>
-      <c r="L4" s="4" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="25" t="inlineStr">
-        <is>
-          <t>DS164 LAB
-C202
-Dr. Siddharth R</t>
-        </is>
-      </c>
-      <c r="O4" s="4" t="n"/>
-      <c r="P4" s="4" t="n"/>
-      <c r="Q4" s="5" t="n"/>
-      <c r="R4" s="7" t="inlineStr"/>
-      <c r="S4" s="7" t="inlineStr"/>
-      <c r="T4" s="7" t="inlineStr"/>
-    </row>
-    <row r="5" ht="40" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
           <t>MA163 LEC
 C204
 Dr. Sibasankar Padhy</t>
         </is>
       </c>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="12" t="inlineStr">
+        <is>
+          <t>CS164 LEC
+L303
+Dr. Manjunath</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="7" t="inlineStr"/>
+      <c r="I4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K4" s="12" t="inlineStr">
+        <is>
+          <t>CS164 LEC
+C203
+Dr. Manjunath</t>
+        </is>
+      </c>
+      <c r="L4" s="4" t="n"/>
+      <c r="M4" s="5" t="n"/>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>HS161 LEC
+C203
+Dr. Rajesh N S</t>
+        </is>
+      </c>
+      <c r="O4" s="4" t="n"/>
+      <c r="P4" s="5" t="n"/>
+      <c r="Q4" s="10" t="inlineStr">
+        <is>
+          <t>CS163 LEC
+C102
+Dr. Sunil Saumya</t>
+        </is>
+      </c>
+      <c r="R4" s="4" t="n"/>
+      <c r="S4" s="5" t="n"/>
+      <c r="T4" s="7" t="inlineStr"/>
+    </row>
+    <row r="5" ht="40" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>HS161 LEC
+C204
+Dr. Rajesh N S</t>
+        </is>
+      </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>MA163 LEC
-L303
-Dr. Sibasankar Padhy</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="5" t="n"/>
+      <c r="E5" s="7" t="inlineStr"/>
+      <c r="F5" s="7" t="inlineStr"/>
+      <c r="G5" s="7" t="inlineStr"/>
       <c r="H5" s="7" t="inlineStr"/>
       <c r="I5" s="8" t="inlineStr">
         <is>
@@ -4783,32 +4759,14 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K5" s="12" t="inlineStr">
-        <is>
-          <t>CS162 LEC
-C203
-Dr. Dibyajyothi Guha</t>
-        </is>
-      </c>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="12" t="inlineStr">
-        <is>
-          <t>CS162 TUT
-C203
-Dr. Dibyajyothi Guha</t>
-        </is>
-      </c>
-      <c r="O5" s="5" t="n"/>
-      <c r="P5" s="13" t="inlineStr">
-        <is>
-          <t>CS164 LEC
-C104
-Dr. Manjunath</t>
-        </is>
-      </c>
-      <c r="Q5" s="4" t="n"/>
-      <c r="R5" s="5" t="n"/>
+      <c r="K5" s="7" t="inlineStr"/>
+      <c r="L5" s="7" t="inlineStr"/>
+      <c r="M5" s="7" t="inlineStr"/>
+      <c r="N5" s="7" t="inlineStr"/>
+      <c r="O5" s="7" t="inlineStr"/>
+      <c r="P5" s="7" t="inlineStr"/>
+      <c r="Q5" s="7" t="inlineStr"/>
+      <c r="R5" s="7" t="inlineStr"/>
       <c r="S5" s="7" t="inlineStr"/>
       <c r="T5" s="7" t="inlineStr"/>
     </row>
@@ -4818,24 +4776,24 @@
           <t>Friday</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>CS164 LEC
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>CS162 LEC
 C204
-Dr. Manjunath</t>
+Dr. Dibyajyothi Guha</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
-      <c r="E6" s="10" t="inlineStr">
-        <is>
-          <t>HS161 LEC
+      <c r="E6" s="11" t="inlineStr">
+        <is>
+          <t>CS162 TUT
 L303
-Dr. Rajesh N S</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="5" t="n"/>
+Dr. Dibyajyothi Guha</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="7" t="inlineStr"/>
       <c r="H6" s="7" t="inlineStr"/>
       <c r="I6" s="8" t="inlineStr">
         <is>
@@ -4847,13 +4805,25 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K6" s="7" t="inlineStr"/>
-      <c r="L6" s="7" t="inlineStr"/>
-      <c r="M6" s="7" t="inlineStr"/>
-      <c r="N6" s="7" t="inlineStr"/>
-      <c r="O6" s="7" t="inlineStr"/>
-      <c r="P6" s="7" t="inlineStr"/>
-      <c r="Q6" s="7" t="inlineStr"/>
+      <c r="K6" s="12" t="inlineStr">
+        <is>
+          <t>CS164 LAB
+C203
+Dr. Manjunath</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="n"/>
+      <c r="M6" s="4" t="n"/>
+      <c r="N6" s="5" t="n"/>
+      <c r="O6" s="10" t="inlineStr">
+        <is>
+          <t>CS163 LEC
+C201
+Dr. Sunil Saumya</t>
+        </is>
+      </c>
+      <c r="P6" s="4" t="n"/>
+      <c r="Q6" s="5" t="n"/>
       <c r="R6" s="7" t="inlineStr"/>
       <c r="S6" s="7" t="inlineStr"/>
       <c r="T6" s="7" t="inlineStr"/>
@@ -5069,22 +5039,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="K4:M4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5234,26 +5204,32 @@
           <t>Monday</t>
         </is>
       </c>
-      <c r="B2" s="12" t="inlineStr">
-        <is>
-          <t>HS206 LEC
+      <c r="B2" s="13" t="inlineStr">
+        <is>
+          <t>MA202 LEC
 L301
-Dr. Navyashree</t>
+Dr. Chinmayananda</t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
-      <c r="E2" s="11" t="inlineStr">
-        <is>
-          <t>CS310 TUT
-L303
-Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
+      <c r="E2" s="13" t="inlineStr">
+        <is>
+          <t>MA202 TUT
+L304
+Dr. Chinmayananda</t>
         </is>
       </c>
       <c r="F2" s="5" t="n"/>
-      <c r="G2" s="7" t="inlineStr"/>
-      <c r="H2" s="7" t="inlineStr"/>
-      <c r="I2" s="7" t="inlineStr"/>
+      <c r="G2" s="12" t="inlineStr">
+        <is>
+          <t>CS204 LEC
+L304
+Dr. Manjunath KV</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="n"/>
+      <c r="I2" s="5" t="n"/>
       <c r="J2" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -5264,9 +5240,15 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L2" s="7" t="inlineStr"/>
-      <c r="M2" s="7" t="inlineStr"/>
-      <c r="N2" s="7" t="inlineStr"/>
+      <c r="L2" s="9" t="inlineStr">
+        <is>
+          <t>DS204 LEC
+C202
+Dr. Animesh Chaturvedi</t>
+        </is>
+      </c>
+      <c r="M2" s="4" t="n"/>
+      <c r="N2" s="5" t="n"/>
       <c r="O2" s="7" t="inlineStr"/>
       <c r="P2" s="7" t="inlineStr"/>
       <c r="Q2" s="7" t="inlineStr"/>
@@ -5282,134 +5264,140 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
+          <t>CS204 LEC
+L301
+Dr. Manjunath KV</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="5" t="n"/>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>DS204 LAB
+L304
+Dr. Animesh Chaturvedi</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="5" t="n"/>
+      <c r="I3" s="7" t="inlineStr"/>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K3" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="L3" s="10" t="inlineStr">
+        <is>
+          <t>CS310 TUT
+C203
+Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="n"/>
+      <c r="N3" s="7" t="inlineStr"/>
+      <c r="O3" s="7" t="inlineStr"/>
+      <c r="P3" s="7" t="inlineStr"/>
+      <c r="Q3" s="7" t="inlineStr"/>
+      <c r="R3" s="7" t="inlineStr"/>
+      <c r="S3" s="7" t="inlineStr"/>
+      <c r="T3" s="7" t="inlineStr"/>
+    </row>
+    <row r="4" ht="40" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t>MA202 LEC
+C205
+Dr. Chinmayananda</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>HS206 LEC
+L304
+Dr. Navyashree</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="12" t="inlineStr">
+        <is>
+          <t>CS204 TUT
+C101
+Dr. Manjunath KV</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="n"/>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>DS204 LEC
+C204
+Dr. Animesh Chaturvedi</t>
+        </is>
+      </c>
+      <c r="M4" s="4" t="n"/>
+      <c r="N4" s="5" t="n"/>
+      <c r="O4" s="25" t="inlineStr">
+        <is>
+          <t>DS205 LEC
+C104
+Mr. Manmohan Singh</t>
+        </is>
+      </c>
+      <c r="P4" s="4" t="n"/>
+      <c r="Q4" s="5" t="n"/>
+      <c r="R4" s="25" t="inlineStr">
+        <is>
+          <t>DS205 LEC
+C104
+Mr. Manmohan Singh</t>
+        </is>
+      </c>
+      <c r="S4" s="4" t="n"/>
+      <c r="T4" s="5" t="n"/>
+    </row>
+    <row r="5" ht="40" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
           <t>HS206 LEC
 C205
 Dr. Navyashree</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="5" t="n"/>
-      <c r="E3" s="13" t="inlineStr">
-        <is>
-          <t>CS204 LEC
-L304
-Dr. Manjunath KV</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="n"/>
-      <c r="G3" s="5" t="n"/>
-      <c r="H3" s="7" t="inlineStr"/>
-      <c r="I3" s="7" t="inlineStr"/>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K3" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="L3" s="10" t="inlineStr">
-        <is>
-          <t>DS204 LAB
-C204
-Dr. Animesh Chaturvedi</t>
-        </is>
-      </c>
-      <c r="M3" s="4" t="n"/>
-      <c r="N3" s="4" t="n"/>
-      <c r="O3" s="5" t="n"/>
-      <c r="P3" s="25" t="inlineStr">
-        <is>
-          <t>DS205 LEC
-C201
-Mr. Manmohan Singh</t>
-        </is>
-      </c>
-      <c r="Q3" s="4" t="n"/>
-      <c r="R3" s="5" t="n"/>
-      <c r="S3" s="7" t="inlineStr"/>
-      <c r="T3" s="7" t="inlineStr"/>
-    </row>
-    <row r="4" ht="40" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>MA202 LEC
-C205
-Dr. Chinmayananda</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>MA202 TUT
-L304
-Dr. Chinmayananda</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
-        <is>
-          <t>DS204 LEC
-L304
-Dr. Animesh Chaturvedi</t>
-        </is>
-      </c>
-      <c r="H4" s="4" t="n"/>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="L4" s="25" t="inlineStr">
-        <is>
-          <t>DS205 LEC
-C203
-Mr. Manmohan Singh</t>
-        </is>
-      </c>
-      <c r="M4" s="4" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="7" t="inlineStr"/>
-      <c r="P4" s="7" t="inlineStr"/>
-      <c r="Q4" s="7" t="inlineStr"/>
-      <c r="R4" s="7" t="inlineStr"/>
-      <c r="S4" s="7" t="inlineStr"/>
-      <c r="T4" s="7" t="inlineStr"/>
-    </row>
-    <row r="5" ht="40" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>MA202 LEC
-C205
-Dr. Chinmayananda</t>
-        </is>
-      </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
-      <c r="E5" s="13" t="inlineStr">
-        <is>
-          <t>CS204 LEC
-L304
-Dr. Manjunath KV</t>
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LEC
+L303
+Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
         </is>
       </c>
       <c r="F5" s="4" t="n"/>
@@ -5426,25 +5414,19 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L5" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LEC
-C204
+      <c r="L5" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LAB
+C203
 Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
         </is>
       </c>
       <c r="M5" s="4" t="n"/>
-      <c r="N5" s="5" t="n"/>
-      <c r="O5" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LAB
-C201
-Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
-        </is>
-      </c>
-      <c r="P5" s="4" t="n"/>
-      <c r="Q5" s="4" t="n"/>
-      <c r="R5" s="5" t="n"/>
+      <c r="N5" s="4" t="n"/>
+      <c r="O5" s="5" t="n"/>
+      <c r="P5" s="7" t="inlineStr"/>
+      <c r="Q5" s="7" t="inlineStr"/>
+      <c r="R5" s="7" t="inlineStr"/>
       <c r="S5" s="7" t="inlineStr"/>
       <c r="T5" s="7" t="inlineStr"/>
     </row>
@@ -5454,32 +5436,20 @@
           <t>Friday</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>CS204 TUT
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>CS310 LEC
 C205
-Dr. Manjunath KV</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="n"/>
-      <c r="D6" s="10" t="inlineStr">
-        <is>
-          <t>DS204 LEC
-L304
-Dr. Animesh Chaturvedi</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="n"/>
-      <c r="F6" s="5" t="n"/>
-      <c r="G6" s="11" t="inlineStr">
-        <is>
-          <t>CS310 LEC
-L304
 Dr. Shirshendu &amp; Dr. Utkarsh Khaire</t>
         </is>
       </c>
-      <c r="H6" s="4" t="n"/>
-      <c r="I6" s="5" t="n"/>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="5" t="n"/>
+      <c r="E6" s="7" t="inlineStr"/>
+      <c r="F6" s="7" t="inlineStr"/>
+      <c r="G6" s="7" t="inlineStr"/>
+      <c r="H6" s="7" t="inlineStr"/>
+      <c r="I6" s="7" t="inlineStr"/>
       <c r="J6" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -5639,22 +5609,22 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="E3:H3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="O4:Q4"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5807,27 +5777,26 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>B1-CS464 LEC
-L302
-Dr. Chinmayanand</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
-      <c r="E2" s="9" t="inlineStr">
-        <is>
-          <t>DS309 LEC
-L304
-Dr. Animesh Chaturvedi</t>
+      <c r="E2" s="11" t="inlineStr">
+        <is>
+          <t>DS306 LEC
+L305
+Dr. Utkarsh Khaire</t>
         </is>
       </c>
       <c r="F2" s="4" t="n"/>
       <c r="G2" s="5" t="n"/>
-      <c r="H2" s="10" t="inlineStr">
-        <is>
-          <t>DS308 TUT
+      <c r="H2" s="12" t="inlineStr">
+        <is>
+          <t>DS307 TUT
 C101
-Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
+Mr. Ram Subramanian</t>
         </is>
       </c>
       <c r="I2" s="5" t="n"/>
@@ -5841,18 +5810,24 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L2" s="13" t="inlineStr">
-        <is>
-          <t>DS307 LEC
+      <c r="L2" s="11" t="inlineStr">
+        <is>
+          <t>DS306 LEC
 C203
-Mr. Ram Subramanian</t>
+Dr. Utkarsh Khaire</t>
         </is>
       </c>
       <c r="M2" s="4" t="n"/>
       <c r="N2" s="5" t="n"/>
-      <c r="O2" s="7" t="inlineStr"/>
-      <c r="P2" s="7" t="inlineStr"/>
-      <c r="Q2" s="7" t="inlineStr"/>
+      <c r="O2" s="9" t="inlineStr">
+        <is>
+          <t>DS308 LEC
+C104
+Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
+        </is>
+      </c>
+      <c r="P2" s="4" t="n"/>
+      <c r="Q2" s="5" t="n"/>
       <c r="R2" s="7" t="inlineStr"/>
       <c r="S2" s="7" t="inlineStr"/>
       <c r="T2" s="7" t="inlineStr"/>
@@ -5865,22 +5840,15 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>B1-CS464 LEC
-L301
-Dr. Chinmayanand</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="5" t="n"/>
-      <c r="E3" s="10" t="inlineStr">
-        <is>
-          <t>DS308 LEC
-L305
-Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="n"/>
-      <c r="G3" s="5" t="n"/>
+      <c r="E3" s="7" t="inlineStr"/>
+      <c r="F3" s="7" t="inlineStr"/>
+      <c r="G3" s="7" t="inlineStr"/>
       <c r="H3" s="7" t="inlineStr"/>
       <c r="I3" s="7" t="inlineStr"/>
       <c r="J3" s="8" t="inlineStr">
@@ -5893,9 +5861,15 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L3" s="7" t="inlineStr"/>
-      <c r="M3" s="7" t="inlineStr"/>
-      <c r="N3" s="7" t="inlineStr"/>
+      <c r="L3" s="13" t="inlineStr">
+        <is>
+          <t>DS309 LEC
+C204
+Dr. Animesh Chaturvedi</t>
+        </is>
+      </c>
+      <c r="M3" s="4" t="n"/>
+      <c r="N3" s="5" t="n"/>
       <c r="O3" s="7" t="inlineStr"/>
       <c r="P3" s="7" t="inlineStr"/>
       <c r="Q3" s="7" t="inlineStr"/>
@@ -5911,82 +5885,86 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>B1-CS464 LEC
-L301
-Dr. Chinmayanand</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="5" t="n"/>
-      <c r="E4" s="12" t="inlineStr">
-        <is>
-          <t>DS306 LEC
-L305
-Dr. Utkarsh Khaire</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="n"/>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="13" t="inlineStr">
-        <is>
-          <t>DS307 TUT
-C101
-Mr. Ram Subramanian</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K4" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="L4" s="13" t="inlineStr">
-        <is>
-          <t>DS307 LEC
-C204
-Mr. Ram Subramanian</t>
-        </is>
-      </c>
-      <c r="M4" s="4" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="10" t="inlineStr">
-        <is>
-          <t>DS308 LEC
-C104
-Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
-        </is>
-      </c>
-      <c r="P4" s="4" t="n"/>
-      <c r="Q4" s="5" t="n"/>
-      <c r="R4" s="7" t="inlineStr"/>
-      <c r="S4" s="7" t="inlineStr"/>
-      <c r="T4" s="7" t="inlineStr"/>
-    </row>
-    <row r="5" ht="40" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>B1-CS464 LEC
-L301
-Dr. Chinmayanand</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="5" t="n"/>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E4" s="13" t="inlineStr">
         <is>
           <t>DS309 LEC
 L305
 Dr. Animesh Chaturvedi</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="11" t="inlineStr">
+        <is>
+          <t>DS306 SS
+C102
+Dr. Utkarsh Khaire</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="n"/>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="L4" s="12" t="inlineStr">
+        <is>
+          <t>DS307 LEC
+C205
+Mr. Ram Subramanian</t>
+        </is>
+      </c>
+      <c r="M4" s="4" t="n"/>
+      <c r="N4" s="5" t="n"/>
+      <c r="O4" s="9" t="inlineStr">
+        <is>
+          <t>DS308 LEC
+C201
+Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
+        </is>
+      </c>
+      <c r="P4" s="4" t="n"/>
+      <c r="Q4" s="5" t="n"/>
+      <c r="R4" s="9" t="inlineStr">
+        <is>
+          <t>DS308 TUT
+C201
+Dr. Abdul Wahid &amp; Dr. Rajendra Hegadi</t>
+        </is>
+      </c>
+      <c r="S4" s="5" t="n"/>
+      <c r="T4" s="7" t="inlineStr"/>
+    </row>
+    <row r="5" ht="40" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">B1 LEC
+</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="5" t="n"/>
+      <c r="E5" s="12" t="inlineStr">
+        <is>
+          <t>DS307 LEC
+L304
+Mr. Ram Subramanian</t>
         </is>
       </c>
       <c r="F5" s="4" t="n"/>
@@ -6003,15 +5981,9 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L5" s="12" t="inlineStr">
-        <is>
-          <t>DS306 LEC
-C205
-Dr. Utkarsh Khaire</t>
-        </is>
-      </c>
-      <c r="M5" s="4" t="n"/>
-      <c r="N5" s="5" t="n"/>
+      <c r="L5" s="7" t="inlineStr"/>
+      <c r="M5" s="7" t="inlineStr"/>
+      <c r="N5" s="7" t="inlineStr"/>
       <c r="O5" s="7" t="inlineStr"/>
       <c r="P5" s="7" t="inlineStr"/>
       <c r="Q5" s="7" t="inlineStr"/>
@@ -6027,29 +5999,22 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>B1-CS464 LEC
-L301
-Dr. Chinmayanand</t>
+          <t xml:space="preserve">B1 LEC
+</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
-      <c r="E6" s="12" t="inlineStr">
-        <is>
-          <t>DS306 SS
-L305
-Dr. Utkarsh Khaire</t>
+      <c r="E6" s="13" t="inlineStr">
+        <is>
+          <t>DS309 SS
+L304
+Dr. Animesh Chaturvedi</t>
         </is>
       </c>
       <c r="F6" s="5" t="n"/>
-      <c r="G6" s="9" t="inlineStr">
-        <is>
-          <t>DS309 SS
-L305
-Dr. Animesh Chaturvedi</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="n"/>
+      <c r="G6" s="7" t="inlineStr"/>
+      <c r="H6" s="7" t="inlineStr"/>
       <c r="I6" s="7" t="inlineStr"/>
       <c r="J6" s="8" t="inlineStr">
         <is>
@@ -6113,17 +6078,17 @@
     <row r="12">
       <c r="A12" s="16" t="inlineStr">
         <is>
-          <t>B1-NEW</t>
+          <t>B2-EC361</t>
         </is>
       </c>
       <c r="B12" s="16" t="inlineStr">
         <is>
-          <t>Large Language Models</t>
+          <t>Introduction to 5G Network</t>
         </is>
       </c>
       <c r="C12" s="16" t="inlineStr">
         <is>
-          <t>Dr. Sunil S</t>
+          <t>Dr. Jagadeesha R Bhat</t>
         </is>
       </c>
       <c r="D12" s="16" t="inlineStr">
@@ -6143,17 +6108,17 @@
     <row r="13">
       <c r="A13" s="16" t="inlineStr">
         <is>
-          <t>B1-CS458</t>
+          <t>B1-NEW</t>
         </is>
       </c>
       <c r="B13" s="16" t="inlineStr">
         <is>
-          <t>Natural Language Processing</t>
+          <t>Large Language Models</t>
         </is>
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>Dr. Krishnendu</t>
+          <t>Dr. Sunil S</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -6203,17 +6168,17 @@
     <row r="15">
       <c r="A15" s="16" t="inlineStr">
         <is>
-          <t>B2-EC361</t>
+          <t>B1-CS458</t>
         </is>
       </c>
       <c r="B15" s="16" t="inlineStr">
         <is>
-          <t>Introduction to 5G Network</t>
+          <t>Natural Language Processing</t>
         </is>
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>Dr. Jagadeesha R Bhat</t>
+          <t>Dr. Krishnendu</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
@@ -6512,17 +6477,17 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="L5:N5"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R4:S4"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6673,19 +6638,19 @@
           <t>Monday</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="13" t="inlineStr">
         <is>
           <t>- LEC
 L303
-Dr. Dibyajyothi Guha</t>
+Dr. Somen Bhattacharjee</t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="E2" s="13" t="inlineStr">
         <is>
           <t>- LEC
-L305
+L401
 Dr. Rajesh N S</t>
         </is>
       </c>
@@ -6702,9 +6667,15 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K2" s="7" t="inlineStr"/>
-      <c r="L2" s="7" t="inlineStr"/>
-      <c r="M2" s="7" t="inlineStr"/>
+      <c r="K2" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+C204
+Dr. Prabhu Prasad</t>
+        </is>
+      </c>
+      <c r="L2" s="4" t="n"/>
+      <c r="M2" s="5" t="n"/>
       <c r="N2" s="7" t="inlineStr"/>
       <c r="O2" s="7" t="inlineStr"/>
       <c r="P2" s="7" t="inlineStr"/>
@@ -6719,22 +6690,22 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>- TUT
-L302
-Dr. Somen Bhattacharjee</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="n"/>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>- LAB
-L401
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+L303
 Dr.Jagadish D N</t>
         </is>
       </c>
-      <c r="E3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="5" t="n"/>
+      <c r="E3" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+L305
+Dr. Rajesh N S</t>
+        </is>
+      </c>
       <c r="F3" s="4" t="n"/>
       <c r="G3" s="5" t="n"/>
       <c r="H3" s="7" t="inlineStr"/>
@@ -6748,34 +6719,22 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K3" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-C205
-Dr. Prabhu Prasad</t>
-        </is>
-      </c>
-      <c r="L3" s="4" t="n"/>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="9" t="inlineStr">
+      <c r="K3" s="13" t="inlineStr">
         <is>
           <t>- LAB
 C205
 Dr. Prabhu Prasad</t>
         </is>
       </c>
-      <c r="O3" s="4" t="n"/>
-      <c r="P3" s="4" t="n"/>
-      <c r="Q3" s="5" t="n"/>
-      <c r="R3" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-C102
-Dr. Sibasankar Padhy</t>
-        </is>
-      </c>
-      <c r="S3" s="4" t="n"/>
-      <c r="T3" s="5" t="n"/>
+      <c r="L3" s="4" t="n"/>
+      <c r="M3" s="4" t="n"/>
+      <c r="N3" s="5" t="n"/>
+      <c r="O3" s="7" t="inlineStr"/>
+      <c r="P3" s="7" t="inlineStr"/>
+      <c r="Q3" s="7" t="inlineStr"/>
+      <c r="R3" s="7" t="inlineStr"/>
+      <c r="S3" s="7" t="inlineStr"/>
+      <c r="T3" s="7" t="inlineStr"/>
     </row>
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -6783,22 +6742,22 @@
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+L302
+Dr. Somen Bhattacharjee</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="13" t="inlineStr">
         <is>
           <t>- TUT
-C201
-Dr. Dibyajyothi Guha</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n"/>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
 L401
-Dr.Jagadish D N</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="n"/>
+Dr. Somen Bhattacharjee</t>
+        </is>
+      </c>
       <c r="F4" s="5" t="n"/>
       <c r="G4" s="7" t="inlineStr"/>
       <c r="H4" s="7" t="inlineStr"/>
@@ -6812,18 +6771,24 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K4" s="9" t="inlineStr">
+      <c r="K4" s="13" t="inlineStr">
         <is>
           <t>- LEC
-C205
-Dr. Prabhu Prasad</t>
+L301
+Dr. Dibyajyothi Guha</t>
         </is>
       </c>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="5" t="n"/>
-      <c r="N4" s="7" t="inlineStr"/>
-      <c r="O4" s="7" t="inlineStr"/>
-      <c r="P4" s="7" t="inlineStr"/>
+      <c r="N4" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+L301
+Dr. Dibyajyothi Guha</t>
+        </is>
+      </c>
+      <c r="O4" s="4" t="n"/>
+      <c r="P4" s="5" t="n"/>
       <c r="Q4" s="7" t="inlineStr"/>
       <c r="R4" s="7" t="inlineStr"/>
       <c r="S4" s="7" t="inlineStr"/>
@@ -6835,83 +6800,77 @@
           <t>Thursday</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="13" t="inlineStr">
+        <is>
+          <t>- TUT
+L302
+Dr. Dibyajyothi Guha</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n"/>
+      <c r="D5" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+L305
+Dr. Prabhu Prasad</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="5" t="n"/>
+      <c r="G5" s="7" t="inlineStr"/>
+      <c r="H5" s="7" t="inlineStr"/>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="J5" s="8" t="inlineStr">
+        <is>
+          <t>BREAK</t>
+        </is>
+      </c>
+      <c r="K5" s="13" t="inlineStr">
+        <is>
+          <t>- LEC
+C204
+Dr. Sibasankar Padhy</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="n"/>
+      <c r="M5" s="5" t="n"/>
+      <c r="N5" s="7" t="inlineStr"/>
+      <c r="O5" s="7" t="inlineStr"/>
+      <c r="P5" s="7" t="inlineStr"/>
+      <c r="Q5" s="7" t="inlineStr"/>
+      <c r="R5" s="7" t="inlineStr"/>
+      <c r="S5" s="7" t="inlineStr"/>
+      <c r="T5" s="7" t="inlineStr"/>
+    </row>
+    <row r="6" ht="40" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
         <is>
           <t>- LEC
 L302
-Dr. Somen Bhattacharjee</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="5" t="n"/>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-L401
-Dr. Dibyajyothi Guha</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="5" t="n"/>
-      <c r="H5" s="7" t="inlineStr"/>
-      <c r="I5" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="J5" s="8" t="inlineStr">
-        <is>
-          <t>BREAK</t>
-        </is>
-      </c>
-      <c r="K5" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-L301
 Dr.Jagadish D N</t>
-        </is>
-      </c>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-L301
-Dr. Rajesh N S</t>
-        </is>
-      </c>
-      <c r="O5" s="4" t="n"/>
-      <c r="P5" s="5" t="n"/>
-      <c r="Q5" s="9" t="inlineStr">
-        <is>
-          <t>- TUT
-C202
-Dr. Sibasankar Padhy</t>
-        </is>
-      </c>
-      <c r="R5" s="5" t="n"/>
-      <c r="S5" s="7" t="inlineStr"/>
-      <c r="T5" s="7" t="inlineStr"/>
-    </row>
-    <row r="6" ht="40" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>- LEC
-L302
-Dr. Somen Bhattacharjee</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
-      <c r="E6" s="7" t="inlineStr"/>
-      <c r="F6" s="7" t="inlineStr"/>
-      <c r="G6" s="7" t="inlineStr"/>
-      <c r="H6" s="7" t="inlineStr"/>
+      <c r="E6" s="13" t="inlineStr">
+        <is>
+          <t>- LAB
+L305
+Dr.Jagadish D N</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="5" t="n"/>
       <c r="I6" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -6922,8 +6881,14 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="K6" s="7" t="inlineStr"/>
-      <c r="L6" s="7" t="inlineStr"/>
+      <c r="K6" s="13" t="inlineStr">
+        <is>
+          <t>- TUT
+C204
+Dr. Sibasankar Padhy</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="n"/>
       <c r="M6" s="7" t="inlineStr"/>
       <c r="N6" s="7" t="inlineStr"/>
       <c r="O6" s="7" t="inlineStr"/>
@@ -7090,21 +7055,21 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="K3:N3"/>
     <mergeCell ref="K4:M4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7257,30 +7222,24 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>EC310 LEC
+          <t xml:space="preserve">MA208 LEC
 L304
-Dr. Prakash Pawar</t>
+Dr. Rajib Sharma/ Rajesh Kumar </t>
         </is>
       </c>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="5" t="n"/>
-      <c r="E2" s="10" t="inlineStr">
-        <is>
-          <t>EC204 LEC
-L401
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>EC204 LAB
+L402
 Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
         </is>
       </c>
       <c r="F2" s="4" t="n"/>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="11" t="inlineStr">
-        <is>
-          <t>HS204 TUT
-C102
-Dr. Anushree Kini</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="n"/>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="7" t="inlineStr"/>
       <c r="J2" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -7291,11 +7250,11 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L2" s="11" t="inlineStr">
-        <is>
-          <t>HS204 LEC
-C204
-Dr. Anushree Kini</t>
+      <c r="L2" s="25" t="inlineStr">
+        <is>
+          <t>HS205 LEC
+C205
+Dr. Jolly Thomas IIT Dharwad</t>
         </is>
       </c>
       <c r="M2" s="4" t="n"/>
@@ -7313,32 +7272,26 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t>EC310 LEC
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>EC204 LEC
 L304
-Dr. Prakash Pawar</t>
+Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
         </is>
       </c>
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="5" t="n"/>
-      <c r="E3" s="10" t="inlineStr">
-        <is>
-          <t>EC204 TUT
-L402
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>EC204 LEC
+L401
 Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
         </is>
       </c>
-      <c r="F3" s="5" t="n"/>
-      <c r="G3" s="25" t="inlineStr">
-        <is>
-          <t>HS205 LEC
-L303
-Dr. Jolly Thomas IIT Dharwad</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="n"/>
-      <c r="I3" s="5" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="7" t="inlineStr"/>
+      <c r="I3" s="7" t="inlineStr"/>
       <c r="J3" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -7349,21 +7302,33 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L3" s="25" t="inlineStr">
-        <is>
-          <t>HS205 LEC
+      <c r="L3" s="10" t="inlineStr">
+        <is>
+          <t>HS204 LEC
 L301
-Dr. Jolly Thomas IIT Dharwad</t>
+Dr. Anushree Kini</t>
         </is>
       </c>
       <c r="M3" s="4" t="n"/>
       <c r="N3" s="5" t="n"/>
-      <c r="O3" s="7" t="inlineStr"/>
-      <c r="P3" s="7" t="inlineStr"/>
-      <c r="Q3" s="7" t="inlineStr"/>
-      <c r="R3" s="7" t="inlineStr"/>
-      <c r="S3" s="7" t="inlineStr"/>
-      <c r="T3" s="7" t="inlineStr"/>
+      <c r="O3" s="10" t="inlineStr">
+        <is>
+          <t>HS204 LEC
+C104
+Dr. Anushree Kini</t>
+        </is>
+      </c>
+      <c r="P3" s="4" t="n"/>
+      <c r="Q3" s="5" t="n"/>
+      <c r="R3" s="25" t="inlineStr">
+        <is>
+          <t>HS205 LEC
+C104
+Dr. Jolly Thomas IIT Dharwad</t>
+        </is>
+      </c>
+      <c r="S3" s="4" t="n"/>
+      <c r="T3" s="5" t="n"/>
     </row>
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -7371,26 +7336,32 @@
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MA208 LEC
-L302
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MA208 TUT
+L303
 Dr. Rajib Sharma/ Rajesh Kumar </t>
         </is>
       </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="13" t="inlineStr">
+      <c r="C4" s="5" t="n"/>
+      <c r="D4" s="11" t="inlineStr">
+        <is>
+          <t>EC205 LAB
+L402
+Dr. Pankaj Kumar</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="12" t="inlineStr">
         <is>
           <t>EC310 TUT
-L402
+C104
 Dr. Prakash Pawar</t>
         </is>
       </c>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="7" t="inlineStr"/>
-      <c r="H4" s="7" t="inlineStr"/>
-      <c r="I4" s="7" t="inlineStr"/>
+      <c r="I4" s="5" t="n"/>
       <c r="J4" s="8" t="inlineStr">
         <is>
           <t>BREAK</t>
@@ -7417,7 +7388,7 @@
           <t>Thursday</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">MA208 LEC
 L303
@@ -7426,22 +7397,22 @@
       </c>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="5" t="n"/>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MA208 TUT
-L402
-Dr. Rajib Sharma/ Rajesh Kumar </t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="12" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>EC205 LEC
-L402
+L401
 Dr. Pankaj Kumar</t>
         </is>
       </c>
-      <c r="H5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="5" t="n"/>
+      <c r="H5" s="9" t="inlineStr">
+        <is>
+          <t>EC204 TUT
+C101
+Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
+        </is>
+      </c>
       <c r="I5" s="5" t="n"/>
       <c r="J5" s="8" t="inlineStr">
         <is>
@@ -7455,23 +7426,23 @@
       </c>
       <c r="L5" s="12" t="inlineStr">
         <is>
-          <t>EC205 LEC
-L302
-Dr. Pankaj Kumar</t>
+          <t>EC310 LEC
+C205
+Dr. Prakash Pawar</t>
         </is>
       </c>
       <c r="M5" s="4" t="n"/>
       <c r="N5" s="5" t="n"/>
       <c r="O5" s="12" t="inlineStr">
         <is>
-          <t>EC205 LAB
-C204
-Dr. Pankaj Kumar</t>
+          <t>EC310 LEC
+C102
+Dr. Prakash Pawar</t>
         </is>
       </c>
       <c r="P5" s="4" t="n"/>
-      <c r="Q5" s="4" t="n"/>
-      <c r="R5" s="5" t="n"/>
+      <c r="Q5" s="5" t="n"/>
+      <c r="R5" s="7" t="inlineStr"/>
       <c r="S5" s="7" t="inlineStr"/>
       <c r="T5" s="7" t="inlineStr"/>
     </row>
@@ -7481,25 +7452,25 @@
           <t>Friday</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
-        <is>
-          <t>EC204 LEC
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>EC205 LEC
 L303
-Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
+Dr. Pankaj Kumar</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="5" t="n"/>
       <c r="E6" s="10" t="inlineStr">
         <is>
-          <t>EC204 LAB
+          <t>HS204 TUT
 L401
-Dr. Somen Bhattacharjee / Dr. Jagadish D N (Lab)</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="4" t="n"/>
-      <c r="H6" s="5" t="n"/>
+Dr. Anushree Kini</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="7" t="inlineStr"/>
+      <c r="H6" s="7" t="inlineStr"/>
       <c r="I6" s="7" t="inlineStr"/>
       <c r="J6" s="8" t="inlineStr">
         <is>
@@ -7511,15 +7482,9 @@
           <t>BREAK</t>
         </is>
       </c>
-      <c r="L6" s="11" t="inlineStr">
-        <is>
-          <t>HS204 LEC
-C202
-Dr. Anushree Kini</t>
-        </is>
-      </c>
-      <c r="M6" s="4" t="n"/>
-      <c r="N6" s="5" t="n"/>
+      <c r="L6" s="7" t="inlineStr"/>
+      <c r="M6" s="7" t="inlineStr"/>
+      <c r="N6" s="7" t="inlineStr"/>
       <c r="O6" s="7" t="inlineStr"/>
       <c r="P6" s="7" t="inlineStr"/>
       <c r="Q6" s="7" t="inlineStr"/>
@@ -7666,24 +7631,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="O5:Q5"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>